<commit_message>
VAR time series experiments
</commit_message>
<xml_diff>
--- a/regression/yearly-props.xlsx
+++ b/regression/yearly-props.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasbudig/Documents/Programmieren/python/attack-hypotheses-generation/regression/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7745AD8-2EC0-C742-8D71-40550B4ED427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -613,8 +607,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,177 +669,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -892,7 +717,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -924,27 +749,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -976,24 +783,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1169,16 +958,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1192,41 +979,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>7.6263107721639646E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C2">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D2">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E2">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>9.5328884652049568E-4</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C3">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D3">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E3">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1234,89 +1021,89 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D4">
-        <v>4.6674445740956822E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E4">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C5">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.9065776930409909E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C6">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D6">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E6">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D7">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E7">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>8.5795996186844616E-3</v>
+        <v>0.00718849840255591</v>
       </c>
       <c r="C8">
-        <v>1.188118811881188E-2</v>
+        <v>0.01014040561622465</v>
       </c>
       <c r="D8">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E8">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1325,265 +1112,265 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>6.6730219256434702E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C10">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D10">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E10">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C11">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D11">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E11">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C12">
-        <v>1.9801980198019798E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D12">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E12">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>5.0524308865586273E-2</v>
+        <v>0.04712460063897764</v>
       </c>
       <c r="C13">
-        <v>2.8712871287128711E-2</v>
+        <v>0.0280811232449298</v>
       </c>
       <c r="D13">
-        <v>2.917152858809802E-2</v>
+        <v>0.03133903133903134</v>
       </c>
       <c r="E13">
-        <v>3.3509700176366841E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.03361344537815126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>4.7664442326024788E-3</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="C14">
-        <v>3.9603960396039596E-3</v>
+        <v>0.00390015600624025</v>
       </c>
       <c r="D14">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E14">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01008403361344538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C15">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D15">
-        <v>9.3348891481913644E-3</v>
+        <v>0.007597340930674264</v>
       </c>
       <c r="E15">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16">
-        <v>5.7197330791229741E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C16">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D16">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E16">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C17">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D17">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B18">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C18">
-        <v>6.9306930693069308E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D18">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E18">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C19">
-        <v>6.9306930693069308E-3</v>
+        <v>0.00702028081123245</v>
       </c>
       <c r="D19">
-        <v>8.1680280046674443E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E19">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B20">
-        <v>2.859866539561487E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C20">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D20">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E20">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01344537815126051</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21">
-        <v>1.9065776930409909E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E21">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B22">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C22">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E22">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B23">
-        <v>3.6224976167778838E-2</v>
+        <v>0.03594249201277955</v>
       </c>
       <c r="C23">
-        <v>2.475247524752475E-2</v>
+        <v>0.02418096723868955</v>
       </c>
       <c r="D23">
-        <v>2.80046674445741E-2</v>
+        <v>0.02659069325735992</v>
       </c>
       <c r="E23">
-        <v>1.6754850088183421E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.02016806722689076</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B24">
-        <v>6.6730219256434702E-3</v>
+        <v>0.00718849840255591</v>
       </c>
       <c r="C24">
-        <v>7.9207920792079209E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D24">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E24">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1591,50 +1378,50 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D25">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E25">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B26">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B27">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C27">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D27">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1642,169 +1429,169 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D28">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E28">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B29">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>1.166861143523921E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E29">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B30">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C30">
-        <v>4.9504950495049514E-3</v>
+        <v>0.00546021840873635</v>
       </c>
       <c r="D30">
-        <v>9.3348891481913644E-3</v>
+        <v>0.008547008547008548</v>
       </c>
       <c r="E30">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B31">
-        <v>9.5328884652049568E-4</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C31">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D31">
-        <v>2.3337222870478411E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E31">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B32">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C32">
-        <v>2.9702970297029699E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D32">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E32">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B33">
-        <v>7.6263107721639646E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C33">
-        <v>1.188118811881188E-2</v>
+        <v>0.01014040561622465</v>
       </c>
       <c r="D33">
-        <v>1.6336056009334889E-2</v>
+        <v>0.0170940170940171</v>
       </c>
       <c r="E33">
-        <v>1.234567901234568E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B34">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C34">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D34">
-        <v>5.8343057176196032E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E34">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B35">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C35">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D35">
-        <v>5.8343057176196032E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E35">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B36">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C36">
-        <v>8.9108910891089101E-3</v>
+        <v>0.009360374414976599</v>
       </c>
       <c r="D36">
-        <v>9.3348891481913644E-3</v>
+        <v>0.01044634377967711</v>
       </c>
       <c r="E36">
-        <v>9.700176366843033E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B37">
-        <v>3.5271687321258342E-2</v>
+        <v>0.03753993610223642</v>
       </c>
       <c r="C37">
-        <v>3.9603960396039598E-2</v>
+        <v>0.03978159126365054</v>
       </c>
       <c r="D37">
-        <v>3.7339556592765458E-2</v>
+        <v>0.03513770180436847</v>
       </c>
       <c r="E37">
-        <v>2.9100529100529099E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.03025210084033613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1815,47 +1602,47 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E38">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B39">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C39">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D39">
-        <v>3.5005834305717621E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E39">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B40">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C40">
-        <v>7.9207920792079209E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D40">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E40">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1866,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E41">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1880,67 +1667,67 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D42">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B43">
-        <v>1.5252621544327929E-2</v>
+        <v>0.01757188498402556</v>
       </c>
       <c r="C43">
-        <v>1.4851485148514851E-2</v>
+        <v>0.0171606864274571</v>
       </c>
       <c r="D43">
-        <v>9.3348891481913644E-3</v>
+        <v>0.0113960113960114</v>
       </c>
       <c r="E43">
-        <v>7.9365079365079361E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B44">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C44">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D44">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E44">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B45">
-        <v>1.048617731172545E-2</v>
+        <v>0.01118210862619808</v>
       </c>
       <c r="C45">
-        <v>4.9504950495049514E-3</v>
+        <v>0.00702028081123245</v>
       </c>
       <c r="D45">
-        <v>1.050175029171529E-2</v>
+        <v>0.00949667616334283</v>
       </c>
       <c r="E45">
-        <v>8.8183421516754845E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -1948,123 +1735,123 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>1.9801980198019798E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D46">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B47">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C47">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D47">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E47">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B48">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C48">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D48">
-        <v>1.166861143523921E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E48">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B49">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B50">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C50">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D50">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E50">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B51">
-        <v>1.5252621544327929E-2</v>
+        <v>0.01357827476038339</v>
       </c>
       <c r="C51">
-        <v>1.089108910891089E-2</v>
+        <v>0.01014040561622465</v>
       </c>
       <c r="D51">
-        <v>1.283547257876313E-2</v>
+        <v>0.01234567901234568</v>
       </c>
       <c r="E51">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B52">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D52">
-        <v>5.8343057176196032E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E52">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B53">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2073,100 +1860,100 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B54">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C54">
-        <v>4.9504950495049514E-3</v>
+        <v>0.00390015600624025</v>
       </c>
       <c r="D54">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E54">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B55">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C55">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D55">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E55">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B56">
-        <v>1.2392755004766441E-2</v>
+        <v>0.01198083067092652</v>
       </c>
       <c r="C56">
-        <v>1.188118811881188E-2</v>
+        <v>0.01014040561622465</v>
       </c>
       <c r="D56">
-        <v>8.1680280046674443E-3</v>
+        <v>0.007597340930674264</v>
       </c>
       <c r="E56">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B57">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C57">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B58">
-        <v>9.5328884652049577E-3</v>
+        <v>0.007987220447284345</v>
       </c>
       <c r="C58">
-        <v>1.5841584158415838E-2</v>
+        <v>0.0140405616224649</v>
       </c>
       <c r="D58">
-        <v>4.6674445740956822E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E58">
-        <v>1.322751322751323E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B59">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2175,61 +1962,61 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B60">
-        <v>6.6730219256434702E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C60">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D60">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E60">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B61">
-        <v>6.6730219256434702E-3</v>
+        <v>0.00718849840255591</v>
       </c>
       <c r="C61">
-        <v>1.5841584158415838E-2</v>
+        <v>0.0187207488299532</v>
       </c>
       <c r="D61">
-        <v>2.567094515752625E-2</v>
+        <v>0.02374169040835708</v>
       </c>
       <c r="E61">
-        <v>2.9982363315696651E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.02521008403361345</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C62">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D62">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E62">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -2237,21 +2024,21 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B64">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2260,231 +2047,231 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B65">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>3.5005834305717621E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E65">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B66">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C66">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D66">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E66">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B67">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B68">
-        <v>6.6730219256434702E-3</v>
+        <v>0.007987220447284345</v>
       </c>
       <c r="C68">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D68">
-        <v>8.1680280046674443E-3</v>
+        <v>0.007597340930674264</v>
       </c>
       <c r="E68">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B69">
-        <v>3.336510962821735E-2</v>
+        <v>0.03115015974440894</v>
       </c>
       <c r="C69">
-        <v>1.8811881188118811E-2</v>
+        <v>0.01794071762870515</v>
       </c>
       <c r="D69">
-        <v>1.283547257876313E-2</v>
+        <v>0.01044634377967711</v>
       </c>
       <c r="E69">
-        <v>1.146384479717813E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01344537815126051</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B70">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C70">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D70">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B71">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D71">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E71">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B72">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C72">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D72">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E72">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B73">
-        <v>8.5795996186844616E-3</v>
+        <v>0.00718849840255591</v>
       </c>
       <c r="C73">
-        <v>4.9504950495049514E-3</v>
+        <v>0.00546021840873635</v>
       </c>
       <c r="D73">
-        <v>1.166861143523921E-2</v>
+        <v>0.0113960113960114</v>
       </c>
       <c r="E73">
-        <v>1.8518518518518521E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01848739495798319</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B74">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B75">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C75">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D75">
-        <v>3.5005834305717621E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E75">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B76">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C76">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D76">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E76">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B77">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C77">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D77">
-        <v>4.6674445740956822E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E77">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
         <v>80</v>
       </c>
@@ -2495,47 +2282,47 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B79">
-        <v>9.5328884652049577E-3</v>
+        <v>0.01038338658146965</v>
       </c>
       <c r="C79">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D79">
-        <v>5.8343057176196032E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E79">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B80">
-        <v>4.38512869399428E-2</v>
+        <v>0.04313099041533546</v>
       </c>
       <c r="C80">
-        <v>2.772277227722772E-2</v>
+        <v>0.0296411856474259</v>
       </c>
       <c r="D80">
-        <v>2.567094515752625E-2</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="E80">
-        <v>2.469135802469136E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.03529411764705882</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
@@ -2546,13 +2333,13 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
@@ -2560,237 +2347,237 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E82">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B83">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C83">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D83">
-        <v>7.0011668611435242E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E83">
-        <v>9.700176366843033E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01176470588235294</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B84">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C84">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D84">
-        <v>4.6674445740956822E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E84">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B85">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C85">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D85">
-        <v>3.5005834305717621E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E85">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B86">
-        <v>4.7664442326024788E-3</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="C86">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D86">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E86">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B87">
-        <v>5.7197330791229741E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C87">
-        <v>9.9009900990099011E-4</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D87">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E87">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B88">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C88">
-        <v>2.9702970297029699E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D88">
-        <v>3.5005834305717621E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E88">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B89">
-        <v>3.8131553860819832E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C89">
-        <v>6.9306930693069308E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D89">
-        <v>7.0011668611435242E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E89">
-        <v>1.146384479717813E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01008403361344538</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B90">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C90">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E90">
-        <v>8.8183421516754845E-3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B91">
-        <v>9.5328884652049568E-4</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C91">
-        <v>3.9603960396039596E-3</v>
+        <v>0.00390015600624025</v>
       </c>
       <c r="D91">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E91">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B92">
-        <v>2.3832221163012389E-2</v>
+        <v>0.0255591054313099</v>
       </c>
       <c r="C92">
-        <v>3.0693069306930689E-2</v>
+        <v>0.0296411856474259</v>
       </c>
       <c r="D92">
-        <v>2.683780630105018E-2</v>
+        <v>0.02754036087369421</v>
       </c>
       <c r="E92">
-        <v>2.645502645502645E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.03025210084033613</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B93">
-        <v>9.5328884652049577E-3</v>
+        <v>0.008785942492012779</v>
       </c>
       <c r="C93">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D93">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E93">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B94">
-        <v>4.0038131553860823E-2</v>
+        <v>0.03913738019169329</v>
       </c>
       <c r="C94">
-        <v>4.7524752475247532E-2</v>
+        <v>0.04758190327613104</v>
       </c>
       <c r="D94">
-        <v>3.8506417736289378E-2</v>
+        <v>0.04083570750237417</v>
       </c>
       <c r="E94">
-        <v>4.4091710758377423E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.03865546218487395</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B95">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C95">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D95">
-        <v>3.5005834305717621E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E95">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
         <v>98</v>
       </c>
@@ -2798,16 +2585,16 @@
         <v>0</v>
       </c>
       <c r="C96">
-        <v>9.9009900990099011E-4</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D96">
-        <v>3.5005834305717621E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E96">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
         <v>99</v>
       </c>
@@ -2815,33 +2602,33 @@
         <v>0</v>
       </c>
       <c r="C97">
-        <v>3.9603960396039596E-3</v>
+        <v>0.00390015600624025</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B98">
-        <v>2.3832221163012389E-2</v>
+        <v>0.0255591054313099</v>
       </c>
       <c r="C98">
-        <v>1.6831683168316829E-2</v>
+        <v>0.015600624024961</v>
       </c>
       <c r="D98">
-        <v>2.2170361726954489E-2</v>
+        <v>0.02089268755935423</v>
       </c>
       <c r="E98">
-        <v>9.700176366843033E-3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01512605042016807</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
         <v>101</v>
       </c>
@@ -2849,67 +2636,67 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <v>1.9801980198019798E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E99">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B100">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C100">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D100">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E100">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B101">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C101">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D101">
-        <v>3.5005834305717621E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E101">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B102">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D102">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E102">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
         <v>105</v>
       </c>
@@ -2917,271 +2704,271 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D103">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B104">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D104">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E104">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B105">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C105">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D105">
         <v>0</v>
       </c>
       <c r="E105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B106">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C106">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D106">
-        <v>5.8343057176196032E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E106">
-        <v>7.9365079365079361E-3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B107">
-        <v>1.048617731172545E-2</v>
+        <v>0.01198083067092652</v>
       </c>
       <c r="C107">
-        <v>8.9108910891089101E-3</v>
+        <v>0.007800312012480499</v>
       </c>
       <c r="D107">
-        <v>8.1680280046674443E-3</v>
+        <v>0.007597340930674264</v>
       </c>
       <c r="E107">
-        <v>1.7636684303350969E-2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01176470588235294</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B108">
-        <v>1.334604385128694E-2</v>
+        <v>0.01277955271565495</v>
       </c>
       <c r="C108">
-        <v>1.386138613861386E-2</v>
+        <v>0.0140405616224649</v>
       </c>
       <c r="D108">
-        <v>1.166861143523921E-2</v>
+        <v>0.01329534662867996</v>
       </c>
       <c r="E108">
-        <v>1.322751322751323E-2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01176470588235294</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B109">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C109">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
       <c r="E109">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B110">
-        <v>5.7197330791229741E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C110">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D110">
-        <v>8.1680280046674443E-3</v>
+        <v>0.008547008547008548</v>
       </c>
       <c r="E110">
-        <v>2.469135802469136E-2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.02352941176470588</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B111">
-        <v>4.7664442326024788E-3</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="C111">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D111">
-        <v>2.3337222870478411E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E111">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B112">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C112">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D112">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E112">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B113">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C113">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D113">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E113">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B114">
-        <v>1.334604385128694E-2</v>
+        <v>0.01277955271565495</v>
       </c>
       <c r="C114">
-        <v>2.9702970297029699E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D114">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E114">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B115">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C115">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D115">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E115">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B116">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C116">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D116">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B117">
-        <v>1.9065776930409909E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C117">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D117">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E117">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B118">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C118">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D118">
-        <v>9.3348891481913644E-3</v>
+        <v>0.007597340930674264</v>
       </c>
       <c r="E118">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="1" t="s">
         <v>121</v>
       </c>
@@ -3189,75 +2976,75 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D119">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E119">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B120">
-        <v>5.7197330791229741E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C120">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D120">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E120">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B121">
-        <v>2.4785510009532889E-2</v>
+        <v>0.02476038338658147</v>
       </c>
       <c r="C121">
-        <v>3.1683168316831677E-2</v>
+        <v>0.031201248049922</v>
       </c>
       <c r="D121">
-        <v>3.5005834305717617E-2</v>
+        <v>0.03513770180436847</v>
       </c>
       <c r="E121">
-        <v>3.7037037037037028E-2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.04033613445378152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B122">
-        <v>1.9065776930409909E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C122">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D122">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E122">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B123">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C123">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -3266,29 +3053,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B124">
-        <v>3.8131553860819832E-3</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="C124">
-        <v>3.9603960396039596E-3</v>
+        <v>0.007800312012480499</v>
       </c>
       <c r="D124">
-        <v>7.0011668611435242E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E124">
-        <v>1.146384479717813E-2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B125">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -3297,44 +3084,44 @@
         <v>0</v>
       </c>
       <c r="E125">
-        <v>7.9365079365079361E-3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B126">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C126">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D126">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E126">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B127">
-        <v>6.6730219256434702E-3</v>
+        <v>0.00718849840255591</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D127">
-        <v>2.3337222870478411E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E127">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="1" t="s">
         <v>130</v>
       </c>
@@ -3342,67 +3129,67 @@
         <v>0</v>
       </c>
       <c r="C128">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D128">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E128">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B129">
-        <v>9.5328884652049568E-4</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C129">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D129">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E129">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B130">
-        <v>2.859866539561487E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C130">
-        <v>5.9405940594059407E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D130">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E130">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B131">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C131">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D131">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E131">
-        <v>8.8183421516754845E-3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="1" t="s">
         <v>134</v>
       </c>
@@ -3410,50 +3197,50 @@
         <v>0</v>
       </c>
       <c r="C132">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D132">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E132">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B133">
-        <v>3.0505243088655858E-2</v>
+        <v>0.03115015974440894</v>
       </c>
       <c r="C133">
-        <v>3.1683168316831677E-2</v>
+        <v>0.0327613104524181</v>
       </c>
       <c r="D133">
-        <v>2.1003500583430569E-2</v>
+        <v>0.02184235517568851</v>
       </c>
       <c r="E133">
-        <v>2.5573192239858909E-2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.03361344537815126</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B134">
-        <v>4.7664442326024788E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C134">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D134">
-        <v>9.3348891481913644E-3</v>
+        <v>0.008547008547008548</v>
       </c>
       <c r="E134">
-        <v>7.9365079365079361E-3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="1" t="s">
         <v>137</v>
       </c>
@@ -3461,118 +3248,118 @@
         <v>0</v>
       </c>
       <c r="C135">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D135">
         <v>0</v>
       </c>
       <c r="E135">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B136">
-        <v>1.143946615824595E-2</v>
+        <v>0.01038338658146965</v>
       </c>
       <c r="C136">
-        <v>6.9306930693069308E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D136">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E136">
-        <v>7.9365079365079361E-3</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01344537815126051</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B137">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C137">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D137">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E137">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5">
       <c r="A138" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B138">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C138">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D138">
-        <v>4.6674445740956822E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E138">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B139">
-        <v>9.5328884652049568E-4</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C139">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0062402496099844</v>
       </c>
       <c r="D139">
-        <v>7.0011668611435242E-3</v>
+        <v>0.007597340930674264</v>
       </c>
       <c r="E139">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B140">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C140">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D140">
         <v>0</v>
       </c>
       <c r="E140">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B141">
-        <v>5.7197330791229741E-3</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="C141">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D141">
         <v>0</v>
       </c>
       <c r="E141">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="1" t="s">
         <v>144</v>
       </c>
@@ -3580,118 +3367,118 @@
         <v>0</v>
       </c>
       <c r="C142">
-        <v>2.9702970297029699E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D142">
-        <v>1.166861143523921E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E142">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B143">
-        <v>1.143946615824595E-2</v>
+        <v>0.01118210862619808</v>
       </c>
       <c r="C143">
-        <v>1.6831683168316829E-2</v>
+        <v>0.015600624024961</v>
       </c>
       <c r="D143">
-        <v>7.0011668611435242E-3</v>
+        <v>0.01044634377967711</v>
       </c>
       <c r="E143">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B144">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D144">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E144">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B145">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C145">
-        <v>2.9702970297029699E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D145">
-        <v>3.5005834305717621E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E145">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B146">
-        <v>7.6263107721639646E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C146">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D146">
-        <v>3.5005834305717621E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E146">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B147">
-        <v>5.7197330791229741E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C147">
-        <v>4.9504950495049514E-3</v>
+        <v>0.00546021840873635</v>
       </c>
       <c r="D147">
-        <v>3.5005834305717621E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E147">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B148">
-        <v>5.7197330791229741E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C148">
         <v>0</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E148">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="1" t="s">
         <v>151</v>
       </c>
@@ -3705,103 +3492,103 @@
         <v>0</v>
       </c>
       <c r="E149">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B150">
-        <v>3.8131553860819832E-3</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D150">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E150">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B151">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C151">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D151">
-        <v>1.166861143523921E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E151">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B152">
-        <v>9.5328884652049577E-3</v>
+        <v>0.007987220447284345</v>
       </c>
       <c r="C152">
-        <v>1.386138613861386E-2</v>
+        <v>0.0140405616224649</v>
       </c>
       <c r="D152">
-        <v>1.6336056009334889E-2</v>
+        <v>0.01424501424501425</v>
       </c>
       <c r="E152">
-        <v>1.322751322751323E-2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01008403361344538</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B153">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C153">
-        <v>3.9603960396039596E-3</v>
+        <v>0.00390015600624025</v>
       </c>
       <c r="D153">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B154">
-        <v>2.0972354623450901E-2</v>
+        <v>0.02236421725239617</v>
       </c>
       <c r="C154">
-        <v>2.2772277227722772E-2</v>
+        <v>0.0234009360374415</v>
       </c>
       <c r="D154">
-        <v>1.9836639439906649E-2</v>
+        <v>0.02089268755935423</v>
       </c>
       <c r="E154">
-        <v>9.700176366843033E-3</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01512605042016807</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B155">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C155">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -3810,7 +3597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5">
       <c r="A156" s="1" t="s">
         <v>158</v>
       </c>
@@ -3821,30 +3608,30 @@
         <v>0</v>
       </c>
       <c r="D156">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E156">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B157">
-        <v>0</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C157">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D157">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E157">
-        <v>3.5273368606701938E-3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158" s="1" t="s">
         <v>160</v>
       </c>
@@ -3852,21 +3639,21 @@
         <v>0</v>
       </c>
       <c r="C158">
-        <v>2.9702970297029699E-3</v>
+        <v>0.00234009360374415</v>
       </c>
       <c r="D158">
-        <v>2.3337222870478411E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E158">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B159">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3875,78 +3662,78 @@
         <v>0</v>
       </c>
       <c r="E159">
-        <v>7.0546737213403876E-3</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160" s="1" t="s">
         <v>162</v>
       </c>
       <c r="B160">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C160">
-        <v>3.9603960396039596E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D160">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E160">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B161">
-        <v>1.143946615824595E-2</v>
+        <v>0.01198083067092652</v>
       </c>
       <c r="C161">
-        <v>1.089108910891089E-2</v>
+        <v>0.008580343213728549</v>
       </c>
       <c r="D161">
-        <v>5.8343057176196032E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E161">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B162">
-        <v>3.8131553860819832E-3</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="C162">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D162">
         <v>0</v>
       </c>
       <c r="E162">
-        <v>4.4091710758377423E-3</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B163">
-        <v>9.5328884652049577E-3</v>
+        <v>0.01118210862619808</v>
       </c>
       <c r="C163">
-        <v>1.386138613861386E-2</v>
+        <v>0.01326053042121685</v>
       </c>
       <c r="D163">
-        <v>8.1680280046674443E-3</v>
+        <v>0.00949667616334283</v>
       </c>
       <c r="E163">
-        <v>8.8183421516754845E-3</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" s="1" t="s">
         <v>166</v>
       </c>
@@ -3960,35 +3747,35 @@
         <v>0</v>
       </c>
       <c r="E164">
-        <v>1.7636684303350969E-3</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B165">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C165">
-        <v>5.9405940594059407E-3</v>
+        <v>0.00546021840873635</v>
       </c>
       <c r="D165">
-        <v>4.6674445740956822E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E165">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B166">
-        <v>1.9065776930409909E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C166">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D166">
         <v>0</v>
@@ -3997,160 +3784,160 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5">
       <c r="A167" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B167">
-        <v>3.5271687321258342E-2</v>
+        <v>0.03913738019169329</v>
       </c>
       <c r="C167">
-        <v>4.8514851485148523E-2</v>
+        <v>0.0483619344773791</v>
       </c>
       <c r="D167">
-        <v>3.3838973162193697E-2</v>
+        <v>0.03513770180436847</v>
       </c>
       <c r="E167">
-        <v>3.7918871252204583E-2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.04201680672268908</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B168">
-        <v>2.0019065776930411E-2</v>
+        <v>0.0207667731629393</v>
       </c>
       <c r="C168">
-        <v>3.2673267326732668E-2</v>
+        <v>0.0327613104524181</v>
       </c>
       <c r="D168">
-        <v>2.3337222870478409E-2</v>
+        <v>0.02279202279202279</v>
       </c>
       <c r="E168">
-        <v>2.1164021164021159E-2</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.02857142857142857</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B169">
-        <v>8.5795996186844616E-3</v>
+        <v>0.008785942492012779</v>
       </c>
       <c r="C169">
-        <v>7.9207920792079209E-3</v>
+        <v>0.008580343213728549</v>
       </c>
       <c r="D169">
-        <v>4.6674445740956822E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E169">
-        <v>7.9365079365079361E-3</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01176470588235294</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B170">
-        <v>1.429933269780744E-2</v>
+        <v>0.01837060702875399</v>
       </c>
       <c r="C170">
-        <v>2.475247524752475E-2</v>
+        <v>0.0249609984399376</v>
       </c>
       <c r="D170">
-        <v>1.9836639439906649E-2</v>
+        <v>0.01994301994301994</v>
       </c>
       <c r="E170">
-        <v>1.8518518518518521E-2</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.02016806722689076</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B171">
-        <v>8.5795996186844616E-3</v>
+        <v>0.009584664536741214</v>
       </c>
       <c r="C171">
-        <v>6.9306930693069308E-3</v>
+        <v>0.009360374414976599</v>
       </c>
       <c r="D171">
-        <v>3.5005834305717621E-3</v>
+        <v>0.004748338081671415</v>
       </c>
       <c r="E171">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B172">
-        <v>5.7197330791229741E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C172">
-        <v>5.9405940594059407E-3</v>
+        <v>0.00546021840873635</v>
       </c>
       <c r="D172">
-        <v>8.1680280046674443E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E172">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B173">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C173">
         <v>0</v>
       </c>
       <c r="D173">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E173">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B174">
-        <v>6.6730219256434702E-3</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="C174">
-        <v>4.9504950495049514E-3</v>
+        <v>0.00546021840873635</v>
       </c>
       <c r="D174">
-        <v>1.050175029171529E-2</v>
+        <v>0.01044634377967711</v>
       </c>
       <c r="E174">
-        <v>6.1728395061728392E-3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.008403361344537815</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B175">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C175">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D175">
-        <v>0</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E175">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
         <v>178</v>
       </c>
@@ -4158,101 +3945,101 @@
         <v>0</v>
       </c>
       <c r="C176">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D176">
         <v>0</v>
       </c>
       <c r="E176">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B177">
-        <v>9.5328884652049568E-4</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C177">
-        <v>1.9801980198019798E-3</v>
+        <v>0.00390015600624025</v>
       </c>
       <c r="D177">
-        <v>7.0011668611435242E-3</v>
+        <v>0.005698005698005698</v>
       </c>
       <c r="E177">
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5">
       <c r="A178" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B178">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C178">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0015600624024961</v>
       </c>
       <c r="D178">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E178">
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5">
       <c r="A179" s="1" t="s">
         <v>181</v>
       </c>
       <c r="B179">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C179">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D179">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E179">
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5">
       <c r="A180" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B180">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C180">
         <v>0</v>
       </c>
       <c r="D180">
-        <v>3.5005834305717621E-3</v>
+        <v>0.002849002849002849</v>
       </c>
       <c r="E180">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B181">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C181">
-        <v>1.9801980198019798E-3</v>
+        <v>0.0031201248049922</v>
       </c>
       <c r="D181">
-        <v>8.1680280046674443E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E181">
-        <v>1.5873015873015869E-2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.01512605042016807</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
       <c r="A182" s="1" t="s">
         <v>184</v>
       </c>
@@ -4260,101 +4047,101 @@
         <v>0</v>
       </c>
       <c r="C182">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D182">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E182">
-        <v>7.0546737213403876E-3</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
       <c r="A183" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B183">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C183">
         <v>0</v>
       </c>
       <c r="D183">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E183">
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5">
       <c r="A184" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B184">
-        <v>9.5328884652049568E-4</v>
+        <v>0.0007987220447284345</v>
       </c>
       <c r="C184">
-        <v>0</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D184">
-        <v>2.3337222870478411E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E184">
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5">
       <c r="A185" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B185">
-        <v>1.9065776930409909E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C185">
-        <v>4.9504950495049514E-3</v>
+        <v>0.0046801872074883</v>
       </c>
       <c r="D185">
-        <v>9.3348891481913644E-3</v>
+        <v>0.00949667616334283</v>
       </c>
       <c r="E185">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.006722689075630253</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
       <c r="A186" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B186">
-        <v>2.859866539561487E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C186">
         <v>0</v>
       </c>
       <c r="D186">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E186">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
       <c r="A187" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B187">
-        <v>1.9065776930409909E-3</v>
+        <v>0.002396166134185303</v>
       </c>
       <c r="C187">
-        <v>6.9306930693069308E-3</v>
+        <v>0.007800312012480499</v>
       </c>
       <c r="D187">
-        <v>7.0011668611435242E-3</v>
+        <v>0.006647673314339981</v>
       </c>
       <c r="E187">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.005042016806722689</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
       <c r="A188" s="1" t="s">
         <v>190</v>
       </c>
@@ -4365,13 +4152,13 @@
         <v>0</v>
       </c>
       <c r="D188">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E188">
-        <v>5.2910052910052907E-3</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.003361344537815126</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
       <c r="A189" s="1" t="s">
         <v>191</v>
       </c>
@@ -4379,55 +4166,55 @@
         <v>0</v>
       </c>
       <c r="C189">
-        <v>9.9009900990099011E-4</v>
+        <v>0.0007800312012480499</v>
       </c>
       <c r="D189">
-        <v>1.166861143523921E-3</v>
+        <v>0.000949667616334283</v>
       </c>
       <c r="E189">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
       <c r="A190" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B190">
-        <v>6.6730219256434702E-3</v>
+        <v>0.005591054313099041</v>
       </c>
       <c r="C190">
-        <v>8.9108910891089101E-3</v>
+        <v>0.007800312012480499</v>
       </c>
       <c r="D190">
-        <v>3.5005834305717621E-3</v>
+        <v>0.003798670465337132</v>
       </c>
       <c r="E190">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
       <c r="A191" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B191">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C191">
         <v>0</v>
       </c>
       <c r="D191">
-        <v>1.166861143523921E-3</v>
+        <v>0.001899335232668566</v>
       </c>
       <c r="E191">
-        <v>2.6455026455026449E-3</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
       <c r="A192" s="1" t="s">
         <v>194</v>
       </c>
       <c r="B192">
-        <v>1.9065776930409909E-3</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -4436,37 +4223,27 @@
         <v>0</v>
       </c>
       <c r="E192">
-        <v>8.8183421516754845E-4</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.001680672268907563</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
       <c r="A193" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B193">
-        <v>4.7664442326024788E-3</v>
+        <v>0.003993610223642172</v>
       </c>
       <c r="C193">
-        <v>1.089108910891089E-2</v>
+        <v>0.01014040561622465</v>
       </c>
       <c r="D193">
-        <v>1.6336056009334889E-2</v>
+        <v>0.01614434947768281</v>
       </c>
       <c r="E193">
-        <v>7.0546737213403876E-3</v>
+        <v>0.003361344537815126</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M164">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0.007</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E193">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0.007</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>